<commit_message>
condenses weather levels in trap metadata and file
</commit_message>
<xml_diff>
--- a/data-raw/metadata/deer_mill_trap_metadata.xlsx
+++ b/data-raw/metadata/deer_mill_trap_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-deer-mill-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-deer-mill-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987E9EB0-E6CC-2840-A8F5-98A9D1647EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB647299-45B2-BA43-A68A-6B1DF33832BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12960" yWindow="620" windowWidth="15840" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -133,9 +133,6 @@
     <t>weather</t>
   </si>
   <si>
-    <t>Description of weather during trap visit. Levels = c("rain", "cloudy", "fog", "partly cloudy", "sunny", "rainy")</t>
-  </si>
-  <si>
     <t>water_temperature</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t>gallon</t>
+  </si>
+  <si>
+    <t>Description of weather during trap visit. Levels = c("cloudy", "fog", "partly cloudy", "sunny", "rainy", "snow")</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -736,7 +736,7 @@
         <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -758,7 +758,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
@@ -806,10 +806,10 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
@@ -824,7 +824,7 @@
         <v>18</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>20</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -28536,13 +28536,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates trap table col names and associated metadata, rewrites xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/deer_mill_trap_metadata.xlsx
+++ b/data-raw/metadata/deer_mill_trap_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-deer-mill-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erincain/Documents/Git/JPE/jpe-deer-mill-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB647299-45B2-BA43-A68A-6B1DF33832BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39605A58-468A-6543-8E40-0D764E6208FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32880" yWindow="-4320" windowWidth="28800" windowHeight="16340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -121,9 +121,6 @@
     <t>Name of stream where sampling site is located</t>
   </si>
   <si>
-    <t>trap_condition_code</t>
-  </si>
-  <si>
     <t>Condition of the trap. Levels = c("normal", "cone stopped", "partial blockage", "total blockage")</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t>Description of weather during trap visit. Levels = c("cloudy", "fog", "partly cloudy", "sunny", "rainy", "snow")</t>
+  </si>
+  <si>
+    <t>trap_condition</t>
   </si>
 </sst>
 </file>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -647,10 +647,10 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -688,7 +688,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
@@ -733,10 +733,10 @@
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -758,7 +758,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
@@ -806,10 +806,10 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
@@ -824,7 +824,7 @@
         <v>18</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>20</v>
@@ -854,7 +854,7 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -28528,7 +28528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABAFE15F-D6B3-E645-9A12-24A655C96D9F}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -28536,13 +28536,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>